<commit_message>
dge on subcluster excluded cells
Former-commit-id: d08fba186a704ae3deff3e83db39b169dae44aa3
</commit_message>
<xml_diff>
--- a/resources/subclusters_removed_byQC_final.xlsx
+++ b/resources/subclusters_removed_byQC_final.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LOChen/orion/nucseq_nd_dpolioud/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE7E310-6BAC-9F40-BBC1-C94E5A0A65A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9A15BD-AA60-9541-9D77-AA638D5A00BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BADcluster_finalList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t>ct_subcluster</t>
   </si>
   <si>
     <t>label</t>
-  </si>
-  <si>
-    <t>calcarine-astrocyte-3</t>
   </si>
   <si>
     <t>calcarine-astrocyte-5</t>
@@ -435,14 +432,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,17 +846,17 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -870,7 +866,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -880,15 +876,15 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -898,121 +894,121 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1022,70 +1018,70 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1104,13 +1100,16 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1118,7 +1117,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1126,20 +1125,20 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B53" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1147,33 +1146,30 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B59" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1187,7 +1183,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1222,7 +1218,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1232,7 +1228,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1242,12 +1238,12 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1262,52 +1258,55 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B78" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="A80" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B80" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="B81" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B82" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1314,7 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1323,7 +1322,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,36 +1330,33 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
         <v>90</v>
       </c>
-      <c r="B88" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="A89" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="B90" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B91" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1369,27 +1365,27 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1404,7 +1400,7 @@
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1414,7 +1410,7 @@
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1434,12 +1430,12 @@
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1465,17 +1461,12 @@
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>